<commit_message>
fixed gantt chart for documentation
</commit_message>
<xml_diff>
--- a/doc/chart/gantt-chart.xlsx
+++ b/doc/chart/gantt-chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Task</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>End Date</t>
-  </si>
-  <si>
-    <t>Add Payment feature with PayPal</t>
   </si>
   <si>
     <t>Setup the back- end, HTTP Server</t>
@@ -42,10 +39,10 @@
     <t>Add User Authentication and Security</t>
   </si>
   <si>
-    <t>Develop Front- End Application with Basic Template and Functionality</t>
+    <t xml:space="preserve">Duration </t>
   </si>
   <si>
-    <t xml:space="preserve">Duration </t>
+    <t>Develop Front- End Application with Basic Template</t>
   </si>
 </sst>
 </file>
@@ -89,21 +86,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -111,23 +102,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,24 +189,63 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -273,6 +288,25 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -315,6 +349,25 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,29 +389,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>In2Indie</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Gantt Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -370,71 +400,78 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Duration (in Months)</c:v>
+            <c:v>Start Date</c:v>
           </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$3:$C$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1-Apr</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25-Mar</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>18-Mar</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>11-Feb</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>28-Jan</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Add Payment feature with PayPal</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Add User Authentication and Security</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Setup PostGreSQL Database Server</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Setup the back- end, HTTP Server</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Develop Front- End Application with Basic Template and Functionality</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Add User Authentication and Security</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Setup PostGreSQL Database Server</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Setup the back- end, HTTP Server</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Develop Front- End Application with Basic Template</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$7</c:f>
+              <c:f>Sheet1!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41723.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41716.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41681.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Duration</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -450,11 +487,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2105612168"/>
-        <c:axId val="2108555432"/>
+        <c:axId val="2092499112"/>
+        <c:axId val="2092756088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105612168"/>
+        <c:axId val="2092499112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,7 +500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108555432"/>
+        <c:crossAx val="2092756088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -471,20 +508,24 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108555432"/>
+        <c:axId val="2092756088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="41770.0"/>
+          <c:min val="41667.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105612168"/>
+        <c:crossAx val="2092499112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10.0"/>
+        <c:minorUnit val="5.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -508,20 +549,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="22" name="Chart 21"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -861,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -877,87 +918,122 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="23">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="36">
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5">
-        <v>41730</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>41765</v>
-      </c>
+    <row r="3" spans="2:5" ht="18">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5" ht="36">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>41723</v>
+      </c>
+      <c r="D4" s="3">
         <v>6</v>
-      </c>
-      <c r="C4" s="5">
-        <v>41723</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2</v>
       </c>
       <c r="E4" s="4">
         <v>41765</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="36">
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
         <v>41716</v>
       </c>
-      <c r="D5" s="2">
-        <v>2</v>
+      <c r="D5" s="3">
+        <v>7</v>
       </c>
       <c r="E5" s="4">
         <v>41765</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="36">
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
         <v>41681</v>
       </c>
-      <c r="D6" s="2">
-        <v>3</v>
+      <c r="D6" s="3">
+        <v>13</v>
       </c>
       <c r="E6" s="4">
         <v>41765</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="72">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:5" ht="54">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>41667</v>
       </c>
-      <c r="D7" s="2">
-        <v>5</v>
+      <c r="D7" s="3">
+        <v>15</v>
       </c>
       <c r="E7" s="4">
         <v>41765</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="D11">
+        <v>41765</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="C12" s="6">
+        <f>DATE(2014,3,25)</f>
+        <v>41723</v>
+      </c>
+      <c r="D12">
+        <v>41723</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="C13" s="6">
+        <f>DATE(2014,3,18)</f>
+        <v>41716</v>
+      </c>
+      <c r="D13">
+        <v>41716</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="C14" s="6">
+        <v>41681</v>
+      </c>
+      <c r="D14">
+        <v>41681</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="C15" s="6">
+        <f>DATE(2014,2,11)</f>
+        <v>41681</v>
+      </c>
+      <c r="D15">
+        <v>41667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>